<commit_message>
recordings deleted, details and scripts updated
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26803"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="5154" documentId="7_{7F2EE577-6552-4DB7-94F7-C16FD42A681E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CDB9C9-A29B-435E-834B-23E1D4EBAE28}"/>
+  <xr:revisionPtr revIDLastSave="5272" documentId="7_{7F2EE577-6552-4DB7-94F7-C16FD42A681E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80523B23-6026-461F-AF21-C2550F2293E5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="5" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Length of measurements" sheetId="1" r:id="rId1"/>
@@ -962,7 +962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1157,6 +1157,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3750,8 +3752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934EF607-4C51-4F4D-B970-F251D79F64F8}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3762,6 +3764,7 @@
     <col min="8" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -3812,47 +3815,47 @@
         <v>57</v>
       </c>
       <c r="B2" s="23">
-        <f>AVERAGE(B11, B19, B27,B35,B43,H11,H19,H27,H35,H43)</f>
-        <v>0.99785999999999997</v>
+        <f>ROUND(AVERAGE(B11, B19, B27,B35,B43,H11,H19,H27,H35,H43),4)</f>
+        <v>0.99790000000000001</v>
       </c>
       <c r="C2" s="23">
-        <f>AVERAGE(C11, C19, C27,C35,C43,I11,I19,I27,I35,I43)</f>
-        <v>0.99758999999999998</v>
+        <f>ROUND(AVERAGE(C11, C19, C27,C35,C43,I11,I19,I27,I35,I43),4)</f>
+        <v>0.99760000000000004</v>
       </c>
       <c r="D2" s="23">
-        <f>AVERAGE(D11, D19, D27,D35,D43,J11,J19,J27,J35,J43)</f>
-        <v>0.99864000000000019</v>
+        <f>ROUND(AVERAGE(D11, D19, D27,D35,D43,J11,J19,J27,J35,J43),4)</f>
+        <v>0.99860000000000004</v>
       </c>
       <c r="E2" s="37">
-        <f>AVERAGE(E11, E19, E27,E35,E43,K11,K19,K27,K35,K43)</f>
+        <f>ROUND(AVERAGE(E11, E19, E27,E35,E43,K11,K19,K27,K35,K43),4)</f>
         <v>0.99570000000000003</v>
       </c>
       <c r="F2">
         <f>ROUND(AVERAGE(B2:E2),4)</f>
-        <v>0.99739999999999995</v>
+        <v>0.99750000000000005</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>57</v>
       </c>
       <c r="I2">
-        <f>STDEV(B11, B19, B27,B35,B43,I11,I19,I27,I35,I43)</f>
-        <v>3.3721737137276408E-3</v>
+        <f>ROUND(STDEV(B11, B19, B27,B35,B43,I11,I19,I27,I35,I43),4)</f>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="J2">
-        <f>STDEV(C11, C19, C27,C35,C43,J11,J19,J27,J35,J43)</f>
-        <v>1.7010127702179086E-3</v>
+        <f>ROUND(STDEV(C11, C19, C27,C35,C43,J11,J19,J27,J35,J43),4)</f>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="K2">
-        <f>STDEV(D11, D19, D27,D35,D43,K11,K19,K27,K35,K43)</f>
-        <v>5.3493094050644811E-3</v>
+        <f>ROUND(STDEV(D11, D19, D27,D35,D43,K11,K19,K27,K35,K43),4)</f>
+        <v>5.3E-3</v>
       </c>
       <c r="L2" s="16">
-        <f>STDEV(E11, E19, E27,E35,E43,L11,L19,L27,L35,L43)</f>
-        <v>2.0034925061557435E-2</v>
+        <f>ROUND(STDEV(E11, E19, E27,E35,E43,L11,L19,L27,L35,L43),4)</f>
+        <v>0.02</v>
       </c>
       <c r="M2">
-        <f>AVERAGE(I2:L2)</f>
-        <v>7.614355237641866E-3</v>
+        <f>ROUND(AVERAGE(I2:L2),4)</f>
+        <v>7.6E-3</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="42" t="s">
@@ -3868,20 +3871,20 @@
         <v>66</v>
       </c>
       <c r="B3" s="23">
-        <f>AVERAGE(B12, B20, B28,B36,B44,H12,H20,H28,H36,H44)</f>
-        <v>0.99795999999999996</v>
+        <f>ROUND(AVERAGE(B12, B20, B28,B36,B44,H12,H20,H28,H36,H44),4)</f>
+        <v>0.998</v>
       </c>
       <c r="C3" s="23">
-        <f>AVERAGE(C12, C20, C28,C36,C44,I12,I20,I28,I36,I44)</f>
-        <v>0.99892999999999998</v>
+        <f>ROUND(AVERAGE(C12, C20, C28,C36,C44,I12,I20,I28,I36,I44),4)</f>
+        <v>0.99890000000000001</v>
       </c>
       <c r="D3" s="23">
-        <f>AVERAGE(D12, D20, D28,D36,D44,J12,J20,J28,J36,J44)</f>
-        <v>0.99702999999999997</v>
+        <f>ROUND(AVERAGE(D12, D20, D28,D36,D44,J12,J20,J28,J36,J44),4)</f>
+        <v>0.997</v>
       </c>
       <c r="E3" s="37">
-        <f>AVERAGE(E12, E20, E28,E36,E44,K12,K20,K28,K36,K44)</f>
-        <v>0.99348999999999987</v>
+        <f>ROUND(AVERAGE(E12, E20, E28,E36,E44,K12,K20,K28,K36,K44),4)</f>
+        <v>0.99350000000000005</v>
       </c>
       <c r="F3">
         <f>ROUND(AVERAGE(B3:E3),4)</f>
@@ -3891,24 +3894,24 @@
         <v>66</v>
       </c>
       <c r="I3">
-        <f>STDEV(B12, B20, B28,B36,B44,I12,I20,I28,I36,I44)</f>
-        <v>1.566453886259592E-3</v>
+        <f>ROUND(STDEV(B12, B20, B28,B36,B44,I12,I20,I28,I36,I44),4)</f>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="J3">
-        <f>STDEV(C12, C20, C28,C36,C44,J12,J20,J28,J36,J44)</f>
-        <v>6.9183813135732875E-3</v>
+        <f>ROUND(STDEV(C12, C20, C28,C36,C44,J12,J20,J28,J36,J44),4)</f>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="K3">
-        <f>STDEV(D12, D20, D28,D36,D44,K12,K20,K28,K36,K44)</f>
-        <v>1.3243681931816062E-2</v>
+        <f>ROUND(STDEV(D12, D20, D28,D36,D44,K12,K20,K28,K36,K44),4)</f>
+        <v>1.32E-2</v>
       </c>
       <c r="L3" s="16">
-        <f>STDEV(E12, E20, E28,E36,E44,L12,L20,L28,L36,L44)</f>
-        <v>2.1784255272507661E-2</v>
+        <f>ROUND(STDEV(E12, E20, E28,E36,E44,L12,L20,L28,L36,L44),4)</f>
+        <v>2.18E-2</v>
       </c>
       <c r="M3">
-        <f>AVERAGE(I3:L3)</f>
-        <v>1.0878193101039151E-2</v>
+        <f>ROUND(AVERAGE(I3:L3),4)</f>
+        <v>1.09E-2</v>
       </c>
       <c r="N3" s="5"/>
     </row>
@@ -3917,20 +3920,20 @@
         <v>76</v>
       </c>
       <c r="B4" s="23">
-        <f>AVERAGE(B13, B21, B29,B37,B45,H13,H21,H29,H37,H45)</f>
-        <v>0.98963999999999996</v>
+        <f>ROUND(AVERAGE(B13, B21, B29,B37,B45,H13,H21,H29,H37,H45),4)</f>
+        <v>0.98960000000000004</v>
       </c>
       <c r="C4" s="23">
-        <f>AVERAGE(C13, C21, C29,C37,C45,I13,I21,I29,I37,I45)</f>
-        <v>0.99855999999999978</v>
+        <f>ROUND(AVERAGE(C13, C21, C29,C37,C45,I13,I21,I29,I37,I45),4)</f>
+        <v>0.99860000000000004</v>
       </c>
       <c r="D4" s="23">
-        <f>AVERAGE(D13, D21, D29,D37,D45,J13,J21,J29,J37,J45)</f>
-        <v>0.99973000000000012</v>
+        <f>ROUND(AVERAGE(D13, D21, D29,D37,D45,J13,J21,J29,J37,J45),4)</f>
+        <v>0.99970000000000003</v>
       </c>
       <c r="E4" s="37">
-        <f>AVERAGE(E13, E21, E29,E37,E45,K13,K21,K29,K37,K45)</f>
-        <v>0.99941999999999998</v>
+        <f>ROUND(AVERAGE(E13, E21, E29,E37,E45,K13,K21,K29,K37,K45),4)</f>
+        <v>0.99939999999999996</v>
       </c>
       <c r="F4">
         <f>ROUND(AVERAGE(B4:E4),4)</f>
@@ -3940,24 +3943,24 @@
         <v>76</v>
       </c>
       <c r="I4">
-        <f>STDEV(B13, B21, B29,B37,B45,I13,I21,I29,I37,I45)</f>
-        <v>1.4944921099379107E-2</v>
+        <f>ROUND(STDEV(B13, B21, B29,B37,B45,I13,I21,I29,I37,I45),4)</f>
+        <v>1.49E-2</v>
       </c>
       <c r="J4">
-        <f>STDEV(C13, C21, C29,C37,C45,J13,J21,J29,J37,J45)</f>
-        <v>2.1280142021247151E-3</v>
+        <f>ROUND(STDEV(C13, C21, C29,C37,C45,J13,J21,J29,J37,J45),4)</f>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="K4">
-        <f>STDEV(D13, D21, D29,D37,D45,K13,K21,K29,K37,K45)</f>
-        <v>5.1865209919558825E-4</v>
+        <f>ROUND(STDEV(D13, D21, D29,D37,D45,K13,K21,K29,K37,K45),4)</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="L4" s="16">
-        <f>STDEV(E13, E21, E29,E37,E45,L13,L21,L29,L37,L45)</f>
-        <v>1.4393285471589379E-3</v>
+        <f>ROUND(STDEV(E13, E21, E29,E37,E45,L13,L21,L29,L37,L45),4)</f>
+        <v>1.4E-3</v>
       </c>
       <c r="M4">
-        <f>AVERAGE(I4:L4)</f>
-        <v>4.7577289869645866E-3</v>
+        <f>ROUND(AVERAGE(I4:L4),4)</f>
+        <v>4.7000000000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3965,19 +3968,19 @@
         <v>81</v>
       </c>
       <c r="B5" s="23">
-        <f>AVERAGE(B14, B22, B30,B38,B46,H14,H22,H30,H38,H46)</f>
-        <v>0.97450000000000014</v>
+        <f>ROUND(AVERAGE(B14, B22, B30,B38,B46,H14,H22,H30,H38,H46),4)</f>
+        <v>0.97450000000000003</v>
       </c>
       <c r="C5" s="23">
-        <f>AVERAGE(C14, C22, C30,C38,C46,I14,I22,I30,I38,I46)</f>
-        <v>0.9987999999999998</v>
+        <f>ROUND(AVERAGE(C14, C22, C30,C38,C46,I14,I22,I30,I38,I46),4)</f>
+        <v>0.99880000000000002</v>
       </c>
       <c r="D5" s="23">
-        <f>AVERAGE(D14, D22, D30,D38,D46,J14,J22,J30,J38,J46)</f>
-        <v>0.99964000000000008</v>
+        <f>ROUND(AVERAGE(D14, D22, D30,D38,D46,J14,J22,J30,J38,J46),4)</f>
+        <v>0.99960000000000004</v>
       </c>
       <c r="E5" s="37">
-        <f>AVERAGE(E14, E22, E30,E38,E46,K14,K22,K30,K38,K46)</f>
+        <f>ROUND(AVERAGE(E14, E22, E30,E38,E46,K14,K22,K30,K38,K46),4)</f>
         <v>0.99939999999999996</v>
       </c>
       <c r="F5">
@@ -3988,24 +3991,24 @@
         <v>81</v>
       </c>
       <c r="I5">
-        <f>STDEV(B14, B22, B30,B38,B46,I14,I22,I30,I38,I46)</f>
-        <v>3.8841960415108921E-2</v>
+        <f>ROUND(STDEV(B14, B22, B30,B38,B46,I14,I22,I30,I38,I46),4)</f>
+        <v>3.8800000000000001E-2</v>
       </c>
       <c r="J5">
-        <f>STDEV(C14, C22, C30,C38,C46,J14,J22,J30,J38,J46)</f>
-        <v>6.5523532668296323E-4</v>
+        <f>ROUND(STDEV(C14, C22, C30,C38,C46,J14,J22,J30,J38,J46),4)</f>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="K5">
-        <f>STDEV(D14, D22, D30,D38,D46,K14,K22,K30,K38,K46)</f>
-        <v>7.530677998103119E-4</v>
+        <f>ROUND(STDEV(D14, D22, D30,D38,D46,K14,K22,K30,K38,K46),4)</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L5" s="16">
-        <f>STDEV(E14, E22, E30,E38,E46,L14,L22,L30,L38,L46)</f>
-        <v>1.8098802907006474E-3</v>
+        <f>ROUND(STDEV(E14, E22, E30,E38,E46,L14,L22,L30,L38,L46),4)</f>
+        <v>1.8E-3</v>
       </c>
       <c r="M5">
-        <f>AVERAGE(I5:L5)</f>
-        <v>1.0515035958075711E-2</v>
+        <f>ROUND(AVERAGE(I5:L5),4)</f>
+        <v>1.0500000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4013,20 +4016,20 @@
         <v>86</v>
       </c>
       <c r="B6" s="23">
-        <f>AVERAGE(B15, B23, B31,B39,B47,H15,H23,H31,H39,H47)</f>
-        <v>0.99874000000000007</v>
+        <f>ROUND(AVERAGE(B15, B23, B31,B39,B47,H15,H23,H31,H39,H47),4)</f>
+        <v>0.99870000000000003</v>
       </c>
       <c r="C6" s="23">
-        <f>AVERAGE(C15, C23, C31,C39,C47,I15,I23,I31,I39,I47)</f>
-        <v>0.99878</v>
+        <f>ROUND(AVERAGE(C15, C23, C31,C39,C47,I15,I23,I31,I39,I47),4)</f>
+        <v>0.99880000000000002</v>
       </c>
       <c r="D6" s="23">
-        <f>AVERAGE(D15, D23, D31,D39,D47,J15,J23,J31,J39,J47)</f>
-        <v>0.99900999999999995</v>
+        <f>ROUND(AVERAGE(D15, D23, D31,D39,D47,J15,J23,J31,J39,J47),4)</f>
+        <v>0.999</v>
       </c>
       <c r="E6" s="37">
-        <f>AVERAGE(E15, E23, E31,E39,E47,K15,K23,K31,K39,K47)</f>
-        <v>0.99740000000000006</v>
+        <f>ROUND(AVERAGE(E15, E23, E31,E39,E47,K15,K23,K31,K39,K47),4)</f>
+        <v>0.99739999999999995</v>
       </c>
       <c r="F6">
         <f>ROUND(AVERAGE(B6:E6),4)</f>
@@ -4036,24 +4039,24 @@
         <v>86</v>
       </c>
       <c r="I6">
-        <f>STDEV(B15, B23, B31,B39,B47,I15,I23,I31,I39,I47)</f>
-        <v>1.3231276078544722E-3</v>
+        <f>ROUND(STDEV(B15, B23, B31,B39,B47,I15,I23,I31,I39,I47),4)</f>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="J6">
-        <f>STDEV(C15, C23, C31,C39,C47,J15,J23,J31,J39,J47)</f>
-        <v>4.5570458267024384E-4</v>
+        <f>ROUND(STDEV(C15, C23, C31,C39,C47,J15,J23,J31,J39,J47),4)</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K6">
-        <f>STDEV(D15, D23, D31,D39,D47,K15,K23,K31,K39,K47)</f>
-        <v>4.0242183506034443E-3</v>
+        <f>ROUND(STDEV(D15, D23, D31,D39,D47,K15,K23,K31,K39,K47),4)</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="L6" s="16">
-        <f>STDEV(E15, E23, E31,E39,E47,L15,L23,L31,L39,L47)</f>
-        <v>3.2260915465415411E-3</v>
+        <f>ROUND(STDEV(E15, E23, E31,E39,E47,L15,L23,L31,L39,L47),4)</f>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="M6">
-        <f>AVERAGE(I6:L6)</f>
-        <v>2.2572855219174254E-3</v>
+        <f>ROUND(AVERAGE(I6:L6),4)</f>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4061,20 +4064,20 @@
         <v>90</v>
       </c>
       <c r="B7" s="38">
-        <f>AVERAGE(B16, B24, B32,B40,B48,H16,H24,H32,H40,H48)</f>
-        <v>0.99849999999999994</v>
+        <f>ROUND(AVERAGE(B16, B24, B32,B40,B48,H16,H24,H32,H40,H48),4)</f>
+        <v>0.99850000000000005</v>
       </c>
       <c r="C7" s="38">
-        <f>AVERAGE(C16, C24, C32,C40,C48,I16,I24,I32,I40,I48)</f>
-        <v>0.9970699999999999</v>
+        <f>ROUND(AVERAGE(C16, C24, C32,C40,C48,I16,I24,I32,I40,I48),4)</f>
+        <v>0.99709999999999999</v>
       </c>
       <c r="D7" s="38">
-        <f>AVERAGE(D16, D24, D32,D40,D48,J16,J24,J32,J40,J48)</f>
-        <v>0.99953000000000003</v>
+        <f>ROUND(AVERAGE(D16, D24, D32,D40,D48,J16,J24,J32,J40,J48),4)</f>
+        <v>0.99950000000000006</v>
       </c>
       <c r="E7" s="39">
-        <f>AVERAGE(E16, E24, E32,E40,E48,K16,K24,K32,K40,K48)</f>
-        <v>0.99921999999999989</v>
+        <f>ROUND(AVERAGE(E16, E24, E32,E40,E48,K16,K24,K32,K40,K48),4)</f>
+        <v>0.99919999999999998</v>
       </c>
       <c r="F7" s="4">
         <f>ROUND(AVERAGE(B7:E7),4)</f>
@@ -4084,24 +4087,24 @@
         <v>90</v>
       </c>
       <c r="I7" s="4">
-        <f>STDEV(B16, B24, B32,B40,B48,I16,I24,I32,I40,I48)</f>
-        <v>3.2703380729079429E-3</v>
+        <f>ROUND(STDEV(B16, B24, B32,B40,B48,I16,I24,I32,I40,I48),4)</f>
+        <v>3.3E-3</v>
       </c>
       <c r="J7" s="4">
-        <f>STDEV(C16, C24, C32,C40,C48,J16,J24,J32,J40,J48)</f>
-        <v>1.8055777776410386E-3</v>
+        <f>ROUND(STDEV(C16, C24, C32,C40,C48,J16,J24,J32,J40,J48),4)</f>
+        <v>1.8E-3</v>
       </c>
       <c r="K7" s="4">
-        <f>STDEV(D16, D24, D32,D40,D48,K16,K24,K32,K40,K48)</f>
-        <v>1.0317191693694869E-3</v>
+        <f>ROUND(STDEV(D16, D24, D32,D40,D48,K16,K24,K32,K40,K48),4)</f>
+        <v>1E-3</v>
       </c>
       <c r="L7" s="26">
-        <f>STDEV(E16, E24, E32,E40,E48,L16,L24,L32,L40,L48)</f>
-        <v>9.5945586430827752E-4</v>
+        <f>ROUND(STDEV(E16, E24, E32,E40,E48,L16,L24,L32,L40,L48),4)</f>
+        <v>1E-3</v>
       </c>
       <c r="M7" s="4">
-        <f>AVERAGE(I7:L7)</f>
-        <v>1.7667727210566864E-3</v>
+        <f>ROUND(AVERAGE(I7:L7),4)</f>
+        <v>1.8E-3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4124,24 +4127,24 @@
       </c>
       <c r="H8" s="16"/>
       <c r="I8">
-        <f>AVERAGE(I2:I7)</f>
-        <v>1.0553162465872947E-2</v>
+        <f>ROUND(AVERAGE(I2:I7),4)</f>
+        <v>1.06E-2</v>
       </c>
       <c r="J8">
-        <f>AVERAGE(J2:J7)</f>
-        <v>2.2773209954850258E-3</v>
+        <f>ROUND(AVERAGE(J2:J7),4)</f>
+        <v>2.3E-3</v>
       </c>
       <c r="K8">
-        <f>AVERAGE(K2:K7)</f>
-        <v>4.1534414593098956E-3</v>
+        <f>ROUND(AVERAGE(K2:K7),4)</f>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="L8" s="16">
-        <f>AVERAGE(L2:L7)</f>
-        <v>8.2089894304624173E-3</v>
+        <f>ROUND(AVERAGE(L2:L7),4)</f>
+        <v>8.2000000000000007E-3</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="E9" s="16"/>
+      <c r="E9" s="86"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="24" t="s">
@@ -5312,8 +5315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E36BA3-36FB-44D3-AD7F-6767E0A98A6E}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5346,25 +5349,25 @@
       <c r="A2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="23">
-        <f>AVERAGE(B11, B19, B27,B35,B43,H11,H19,H27,H35,H43)</f>
-        <v>1.6706800000000002</v>
-      </c>
-      <c r="C2" s="23">
-        <f>AVERAGE(C11, C19, C27,C35,C43,I11,I19,I27,I35,I43)</f>
+      <c r="B2" s="87">
+        <f>ROUND(AVERAGE(B11, B19, B27,B35,B43,H11,H19,H27,H35,H43),4)</f>
+        <v>1.6707000000000001</v>
+      </c>
+      <c r="C2" s="87">
+        <f>ROUND(AVERAGE(C11, C19, C27,C35,C43,I11,I19,I27,I35,I43),4)</f>
         <v>1.5059</v>
       </c>
-      <c r="D2" s="23">
-        <f>AVERAGE(D11, D19, D27,D35,D43,J11,J19,J27,J35,J43)</f>
-        <v>1.55247</v>
+      <c r="D2" s="87">
+        <f>ROUND(AVERAGE(D11, D19, D27,D35,D43,J11,J19,J27,J35,J43),4)</f>
+        <v>1.5525</v>
       </c>
       <c r="E2" s="37">
-        <f>AVERAGE(E11, E19, E27,E35,E43,K11,K19,K27,K35,K43)</f>
-        <v>1.5823400000000001</v>
+        <f>ROUND(AVERAGE(E11, E19, E27,E35,E43,K11,K19,K27,K35,K43),4)</f>
+        <v>1.5823</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(B2:E2)</f>
-        <v>1.5778475000000003</v>
+        <f>ROUND(AVERAGE(B2:E2),4)</f>
+        <v>1.5779000000000001</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
@@ -5376,25 +5379,25 @@
       <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="23">
-        <f>AVERAGE(B12, B20, B28,B36,B44,H12,H20,H28,H36,H44)</f>
-        <v>1.6707100000000001</v>
-      </c>
-      <c r="C3" s="23">
-        <f>AVERAGE(C12, C20, C28,C36,C44,I12,I20,I28,I36,I44)</f>
-        <v>1.5008500000000002</v>
-      </c>
-      <c r="D3" s="23">
-        <f>AVERAGE(D12, D20, D28,D36,D44,J12,J20,J28,J36,J44)</f>
-        <v>1.54911</v>
+      <c r="B3" s="87">
+        <f>ROUND(AVERAGE(B12, B20, B28,B36,B44,H12,H20,H28,H36,H44),4)</f>
+        <v>1.6707000000000001</v>
+      </c>
+      <c r="C3" s="87">
+        <f>ROUND(AVERAGE(C12, C20, C28,C36,C44,I12,I20,I28,I36,I44),4)</f>
+        <v>1.5008999999999999</v>
+      </c>
+      <c r="D3" s="87">
+        <f>ROUND(AVERAGE(D12, D20, D28,D36,D44,J12,J20,J28,J36,J44),4)</f>
+        <v>1.5490999999999999</v>
       </c>
       <c r="E3" s="37">
-        <f>AVERAGE(E12, E20, E28,E36,E44,K12,K20,K28,K36,K44)</f>
-        <v>1.5811699999999997</v>
+        <f>ROUND(AVERAGE(E12, E20, E28,E36,E44,K12,K20,K28,K36,K44),4)</f>
+        <v>1.5811999999999999</v>
       </c>
       <c r="F3">
-        <f>AVERAGE(B3:E3)</f>
-        <v>1.5754600000000001</v>
+        <f>ROUND(AVERAGE(B3:E3),4)</f>
+        <v>1.5754999999999999</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
@@ -5405,25 +5408,25 @@
       <c r="A4" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="23">
-        <f>AVERAGE(B13, B21, B29,B37,B45,H13,H21,H29,H37,H45)</f>
-        <v>1.6493499999999996</v>
-      </c>
-      <c r="C4" s="23">
-        <f>AVERAGE(C13, C21, C29,C37,C45,I13,I21,I29,I37,I45)</f>
-        <v>1.5038100000000001</v>
-      </c>
-      <c r="D4" s="23">
-        <f>AVERAGE(D13, D21, D29,D37,D45,J13,J21,J29,J37,J45)</f>
-        <v>1.5522800000000001</v>
+      <c r="B4" s="87">
+        <f>ROUND(AVERAGE(B13, B21, B29,B37,B45,H13,H21,H29,H37,H45),4)</f>
+        <v>1.6494</v>
+      </c>
+      <c r="C4" s="87">
+        <f>ROUND(AVERAGE(C13, C21, C29,C37,C45,I13,I21,I29,I37,I45),4)</f>
+        <v>1.5038</v>
+      </c>
+      <c r="D4" s="87">
+        <f>ROUND(AVERAGE(D13, D21, D29,D37,D45,J13,J21,J29,J37,J45),4)</f>
+        <v>1.5523</v>
       </c>
       <c r="E4" s="37">
-        <f>AVERAGE(E13, E21, E29,E37,E45,K13,K21,K29,K37,K45)</f>
-        <v>1.5732900000000001</v>
+        <f>ROUND(AVERAGE(E13, E21, E29,E37,E45,K13,K21,K29,K37,K45),4)</f>
+        <v>1.5732999999999999</v>
       </c>
       <c r="F4">
-        <f>AVERAGE(B4:E4)</f>
-        <v>1.5696824999999999</v>
+        <f>ROUND(AVERAGE(B4:E4),4)</f>
+        <v>1.5697000000000001</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
@@ -5434,25 +5437,25 @@
       <c r="A5" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="23">
-        <f>AVERAGE(B14, B22, B30,B38,B46,H14,H22,H30,H38,H46)</f>
-        <v>1.6477700000000002</v>
-      </c>
-      <c r="C5" s="23">
-        <f>AVERAGE(C14, C22, C30,C38,C46,I14,I22,I30,I38,I46)</f>
-        <v>1.50274</v>
-      </c>
-      <c r="D5" s="23">
-        <f>AVERAGE(D14, D22, D30,D38,D46,J14,J22,J30,J38,J46)</f>
-        <v>1.55121</v>
+      <c r="B5" s="87">
+        <f>ROUND(AVERAGE(B14, B22, B30,B38,B46,H14,H22,H30,H38,H46),4)</f>
+        <v>1.6477999999999999</v>
+      </c>
+      <c r="C5" s="87">
+        <f>ROUND(AVERAGE(C14, C22, C30,C38,C46,I14,I22,I30,I38,I46),4)</f>
+        <v>1.5026999999999999</v>
+      </c>
+      <c r="D5" s="87">
+        <f>ROUND(AVERAGE(D14, D22, D30,D38,D46,J14,J22,J30,J38,J46),4)</f>
+        <v>1.5511999999999999</v>
       </c>
       <c r="E5" s="37">
-        <f>AVERAGE(E14, E22, E30,E38,E46,K14,K22,K30,K38,K46)</f>
-        <v>1.5726899999999999</v>
+        <f>ROUND(AVERAGE(E14, E22, E30,E38,E46,K14,K22,K30,K38,K46),4)</f>
+        <v>1.5727</v>
       </c>
       <c r="F5">
-        <f>AVERAGE(B5:E5)</f>
-        <v>1.5686024999999999</v>
+        <f>ROUND(AVERAGE(B5:E5),4)</f>
+        <v>1.5686</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -5463,25 +5466,25 @@
       <c r="A6" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="23">
-        <f>AVERAGE(B15, B23, B31,B39,B47,H15,H23,H31,H39,H47)</f>
-        <v>1.6722300000000001</v>
-      </c>
-      <c r="C6" s="23">
-        <f>AVERAGE(C15, C23, C31,C39,C47,I15,I23,I31,I39,I47)</f>
-        <v>1.5038999999999998</v>
-      </c>
-      <c r="D6" s="23">
-        <f>AVERAGE(D15, D23, D31,D39,D47,J15,J23,J31,J39,J47)</f>
-        <v>1.5523899999999997</v>
+      <c r="B6" s="87">
+        <f>ROUND(AVERAGE(B15, B23, B31,B39,B47,H15,H23,H31,H39,H47),4)</f>
+        <v>1.6721999999999999</v>
+      </c>
+      <c r="C6" s="87">
+        <f>ROUND(AVERAGE(C15, C23, C31,C39,C47,I15,I23,I31,I39,I47),4)</f>
+        <v>1.5039</v>
+      </c>
+      <c r="D6" s="87">
+        <f>ROUND(AVERAGE(D15, D23, D31,D39,D47,J15,J23,J31,J39,J47),4)</f>
+        <v>1.5524</v>
       </c>
       <c r="E6" s="37">
-        <f>AVERAGE(E15, E23, E31,E39,E47,K15,K23,K31,K39,K47)</f>
-        <v>1.5790900000000003</v>
+        <f>ROUND(AVERAGE(E15, E23, E31,E39,E47,K15,K23,K31,K39,K47),4)</f>
+        <v>1.5790999999999999</v>
       </c>
       <c r="F6">
-        <f>AVERAGE(B6:E6)</f>
-        <v>1.5769025000000001</v>
+        <f>ROUND(AVERAGE(B6:E6),4)</f>
+        <v>1.5769</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -5493,24 +5496,24 @@
         <v>90</v>
       </c>
       <c r="B7" s="38">
-        <f>AVERAGE(B16, B24, B32,B40,B48,H16,H24,H32,H40,H48)</f>
-        <v>1.6413500000000003</v>
+        <f>ROUND(AVERAGE(B16, B24, B32,B40,B48,H16,H24,H32,H40,H48),4)</f>
+        <v>1.6414</v>
       </c>
       <c r="C7" s="38">
-        <f>AVERAGE(C16, C24, C32,C40,C48,I16,I24,I32,I40,I48)</f>
-        <v>1.5006200000000001</v>
+        <f>ROUND(AVERAGE(C16, C24, C32,C40,C48,I16,I24,I32,I40,I48),4)</f>
+        <v>1.5005999999999999</v>
       </c>
       <c r="D7" s="38">
-        <f>AVERAGE(D16, D24, D32,D40,D48,J16,J24,J32,J40,J48)</f>
-        <v>1.5478600000000002</v>
+        <f>ROUND(AVERAGE(D16, D24, D32,D40,D48,J16,J24,J32,J40,J48),4)</f>
+        <v>1.5479000000000001</v>
       </c>
       <c r="E7" s="39">
-        <f>AVERAGE(E16, E24, E32,E40,E48,K16,K24,K32,K40,K48)</f>
-        <v>1.57443</v>
+        <f>ROUND(AVERAGE(E16, E24, E32,E40,E48,K16,K24,K32,K40,K48),4)</f>
+        <v>1.5744</v>
       </c>
       <c r="F7" s="4">
-        <f>AVERAGE(B7:E7)</f>
-        <v>1.566065</v>
+        <f>ROUND(AVERAGE(B7:E7),4)</f>
+        <v>1.5661</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
@@ -5520,20 +5523,20 @@
     <row r="8" spans="1:13">
       <c r="A8" s="16"/>
       <c r="B8">
-        <f>AVERAGE(B2:B7)</f>
-        <v>1.6586816666666671</v>
+        <f>ROUND(AVERAGE(B2:B7),4)</f>
+        <v>1.6587000000000001</v>
       </c>
       <c r="C8">
-        <f>AVERAGE(C2:C7)</f>
-        <v>1.5029700000000001</v>
+        <f>ROUND(AVERAGE(C2:C7),4)</f>
+        <v>1.5029999999999999</v>
       </c>
       <c r="D8">
-        <f>AVERAGE(D2:D7)</f>
-        <v>1.5508866666666667</v>
+        <f>ROUND(AVERAGE(D2:D7),4)</f>
+        <v>1.5508999999999999</v>
       </c>
       <c r="E8" s="16">
-        <f>AVERAGE(E2:E7)</f>
-        <v>1.5771683333333331</v>
+        <f>ROUND(AVERAGE(E2:E7),4)</f>
+        <v>1.5771999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:13">

</xml_diff>